<commit_message>
rename the heroskill to heropower
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/TreasureWheel.xlsx
+++ b/ConfigData/Xlsx/TreasureWheel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -796,46 +796,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -917,76 +877,48 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1044,794 +976,754 @@
         </row>
         <row r="5">
           <cell r="A5">
-            <v>22031002</v>
+            <v>22031101</v>
           </cell>
           <cell r="B5" t="str">
-            <v>卡牌补给包（无）</v>
+            <v>素材袋</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6">
-            <v>22031003</v>
+            <v>22031102</v>
           </cell>
           <cell r="B6" t="str">
-            <v>卡牌补给包（水）</v>
+            <v>高级素材袋</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7">
-            <v>22031004</v>
+            <v>22031103</v>
           </cell>
           <cell r="B7" t="str">
-            <v>卡牌补给包（风）</v>
+            <v>特级素材袋</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8">
-            <v>22031005</v>
+            <v>22031104</v>
           </cell>
           <cell r="B8" t="str">
-            <v>卡牌补给包（地）</v>
+            <v>极品素材袋</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9">
-            <v>22031006</v>
+            <v>22031201</v>
           </cell>
           <cell r="B9" t="str">
-            <v>卡牌补给包（火）</v>
+            <v>蓝色卡包</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10">
-            <v>22031007</v>
+            <v>22031202</v>
           </cell>
           <cell r="B10" t="str">
-            <v>卡牌补给包（光）</v>
+            <v>黄色卡包</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11">
-            <v>22031008</v>
+            <v>22031203</v>
           </cell>
           <cell r="B11" t="str">
-            <v>卡牌补给包（暗）</v>
+            <v>红色卡包</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12">
-            <v>22031011</v>
+            <v>22031212</v>
           </cell>
           <cell r="B12" t="str">
-            <v>卡牌补给包（生物）</v>
+            <v>卡牌补给包（无）</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>22031012</v>
+            <v>22031213</v>
           </cell>
           <cell r="B13" t="str">
-            <v>卡牌补给包（武器）</v>
+            <v>卡牌补给包（水）</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>22031013</v>
+            <v>22031214</v>
           </cell>
           <cell r="B14" t="str">
-            <v>卡牌补给包（法术）</v>
+            <v>卡牌补给包（风）</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>22031101</v>
+            <v>22031215</v>
           </cell>
           <cell r="B15" t="str">
-            <v>资源袋(植物)</v>
+            <v>卡牌补给包（地）</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>22031102</v>
+            <v>22031216</v>
           </cell>
           <cell r="B16" t="str">
-            <v>资源袋(鱼)</v>
+            <v>卡牌补给包（火）</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>22031103</v>
+            <v>22031217</v>
           </cell>
           <cell r="B17" t="str">
-            <v>资源袋(矿石)</v>
+            <v>卡牌补给包（光）</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>22031201</v>
+            <v>22031218</v>
           </cell>
           <cell r="B18" t="str">
-            <v>蓝色卡包</v>
+            <v>卡牌补给包（暗）</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>22031202</v>
+            <v>22031221</v>
           </cell>
           <cell r="B19" t="str">
-            <v>黄色卡包</v>
+            <v>卡牌补给包（生物）</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>22031203</v>
+            <v>22031222</v>
           </cell>
           <cell r="B20" t="str">
-            <v>红色卡包</v>
+            <v>卡牌补给包（武器）</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21">
-            <v>22032001</v>
+            <v>22031223</v>
           </cell>
           <cell r="B21" t="str">
-            <v>木材补给车</v>
+            <v>卡牌补给包（法术）</v>
           </cell>
         </row>
         <row r="22">
           <cell r="A22">
-            <v>22032002</v>
+            <v>22031301</v>
           </cell>
           <cell r="B22" t="str">
-            <v>矿石补给车</v>
+            <v>资源袋(绿)</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>22032003</v>
+            <v>22031302</v>
           </cell>
           <cell r="B23" t="str">
-            <v>水银补给车</v>
+            <v>资源袋(蓝)</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>22032004</v>
+            <v>22031303</v>
           </cell>
           <cell r="B24" t="str">
-            <v>红宝石补给车</v>
+            <v>资源袋(红)</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>22032005</v>
+            <v>22031304</v>
           </cell>
           <cell r="B25" t="str">
-            <v>硫磺补给车</v>
+            <v>资源袋(紫)</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>22032006</v>
+            <v>22031305</v>
           </cell>
           <cell r="B26" t="str">
-            <v>水晶补给车</v>
+            <v>资源袋(灰)</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>22032007</v>
+            <v>22031401</v>
           </cell>
           <cell r="B27" t="str">
-            <v>初始资源包</v>
+            <v>素材袋(无)</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28">
-            <v>22032008</v>
+            <v>22031402</v>
           </cell>
           <cell r="B28" t="str">
-            <v>金币</v>
+            <v>素材袋(水)</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>22033001</v>
+            <v>22031403</v>
           </cell>
           <cell r="B29" t="str">
-            <v>小型魔法药剂</v>
+            <v>素材袋(风)</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30">
-            <v>22033002</v>
+            <v>22031404</v>
           </cell>
           <cell r="B30" t="str">
-            <v>中型魔法药剂</v>
+            <v>素材袋(火)</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31">
-            <v>22033003</v>
+            <v>22031405</v>
           </cell>
           <cell r="B31" t="str">
-            <v>大型魔法药剂</v>
+            <v>素材袋(地)</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32">
-            <v>22033004</v>
+            <v>22031406</v>
           </cell>
           <cell r="B32" t="str">
-            <v>小型活力药剂</v>
+            <v>素材袋(光)</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33">
-            <v>22033005</v>
+            <v>22031407</v>
           </cell>
           <cell r="B33" t="str">
-            <v>中型活力药剂</v>
+            <v>素材袋(暗)</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>22033006</v>
+            <v>22031501</v>
           </cell>
           <cell r="B34" t="str">
-            <v>大型活力药剂</v>
+            <v>资源袋(恶魔)</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35">
-            <v>22033007</v>
+            <v>22031502</v>
           </cell>
           <cell r="B35" t="str">
-            <v>小型体力药剂</v>
+            <v>资源袋(机械)</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36">
-            <v>22033008</v>
+            <v>22031503</v>
           </cell>
           <cell r="B36" t="str">
-            <v>中型体力药剂</v>
+            <v>资源袋(精灵)</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37">
-            <v>22033009</v>
+            <v>22031504</v>
           </cell>
           <cell r="B37" t="str">
-            <v>大型体力药剂</v>
+            <v>资源袋(昆虫)</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>22033013</v>
+            <v>22031505</v>
           </cell>
           <cell r="B38" t="str">
-            <v>随机幻兽卡</v>
+            <v>资源袋(龙)</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39">
-            <v>22033014</v>
+            <v>22031506</v>
           </cell>
           <cell r="B39" t="str">
-            <v>随机武器卡</v>
+            <v>资源袋(鸟)</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>22033015</v>
+            <v>22031507</v>
           </cell>
           <cell r="B40" t="str">
-            <v>随机魔法卡</v>
+            <v>资源袋(爬行)</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>22033016</v>
+            <v>22031508</v>
           </cell>
           <cell r="B41" t="str">
-            <v>符文-查姆</v>
+            <v>资源袋(人类)</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>22033017</v>
+            <v>22031509</v>
           </cell>
           <cell r="B42" t="str">
-            <v>符文-普尔</v>
+            <v>资源袋(兽人)</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>22033018</v>
+            <v>22031510</v>
           </cell>
           <cell r="B43" t="str">
-            <v>符文-艾尔</v>
+            <v>资源袋(亡灵)</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44">
-            <v>22033030</v>
+            <v>22031511</v>
           </cell>
           <cell r="B44" t="str">
-            <v>木质修理锤</v>
+            <v>资源袋(野兽)</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45">
-            <v>22033031</v>
+            <v>22031512</v>
           </cell>
           <cell r="B45" t="str">
-            <v>钢铁修理锤</v>
+            <v>资源袋(鱼)</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>22033032</v>
+            <v>22031513</v>
           </cell>
           <cell r="B46" t="str">
-            <v>神圣修理锤</v>
+            <v>资源袋(元素)</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47">
-            <v>22034001</v>
+            <v>22031514</v>
           </cell>
           <cell r="B47" t="str">
-            <v>经验之书</v>
+            <v>资源袋(植物)</v>
           </cell>
         </row>
         <row r="48">
           <cell r="A48">
-            <v>22034002</v>
+            <v>22031515</v>
           </cell>
           <cell r="B48" t="str">
-            <v>能量之书</v>
+            <v>资源袋(地精)</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>22034003</v>
+            <v>22031516</v>
           </cell>
           <cell r="B49" t="str">
-            <v>攻速药水</v>
+            <v>资源袋(石像)</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>22034004</v>
+            <v>22032001</v>
           </cell>
           <cell r="B50" t="str">
-            <v>守护药水</v>
+            <v>木材补给车</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>22034005</v>
+            <v>22032002</v>
           </cell>
           <cell r="B51" t="str">
-            <v>法术药水</v>
+            <v>矿石补给车</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>22034006</v>
+            <v>22032003</v>
           </cell>
           <cell r="B52" t="str">
-            <v>技巧药水</v>
+            <v>水银补给车</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>22034007</v>
+            <v>22032004</v>
           </cell>
           <cell r="B53" t="str">
-            <v>速度药水</v>
+            <v>红宝石补给车</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>22034008</v>
+            <v>22032005</v>
           </cell>
           <cell r="B54" t="str">
-            <v>幸运药水</v>
+            <v>硫磺补给车</v>
           </cell>
         </row>
         <row r="55">
           <cell r="A55">
-            <v>22034009</v>
+            <v>22032006</v>
           </cell>
           <cell r="B55" t="str">
-            <v>暴击药水</v>
+            <v>水晶补给车</v>
           </cell>
         </row>
         <row r="56">
           <cell r="A56">
-            <v>22034010</v>
+            <v>22032007</v>
           </cell>
           <cell r="B56" t="str">
-            <v>生存药水</v>
+            <v>初始资源包</v>
           </cell>
         </row>
         <row r="57">
           <cell r="A57">
-            <v>22034011</v>
+            <v>22032008</v>
           </cell>
           <cell r="B57" t="str">
-            <v>体力药水</v>
+            <v>金币</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>22035001</v>
+            <v>22033001</v>
           </cell>
           <cell r="B58" t="str">
-            <v>猛兽卡片</v>
+            <v>小型魔法药剂</v>
           </cell>
         </row>
         <row r="59">
           <cell r="A59">
-            <v>22035002</v>
+            <v>22033002</v>
           </cell>
           <cell r="B59" t="str">
-            <v>战斧卡片</v>
+            <v>中型魔法药剂</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>22035003</v>
+            <v>22033003</v>
           </cell>
           <cell r="B60" t="str">
-            <v>火焰卡片</v>
+            <v>大型魔法药剂</v>
           </cell>
         </row>
         <row r="61">
           <cell r="A61">
-            <v>22036101</v>
+            <v>22033004</v>
           </cell>
           <cell r="B61" t="str">
-            <v>名片-塞尼斯</v>
+            <v>小型活力药剂</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>22036102</v>
+            <v>22033005</v>
           </cell>
           <cell r="B62" t="str">
-            <v>名片-塞巴斯恰恩</v>
+            <v>中型活力药剂</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>22036103</v>
+            <v>22033006</v>
           </cell>
           <cell r="B63" t="str">
-            <v>名片-科迪</v>
+            <v>大型活力药剂</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>22036104</v>
+            <v>22033007</v>
           </cell>
           <cell r="B64" t="str">
-            <v>名片-威阿伊丁</v>
+            <v>小型体力药剂</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>22036105</v>
+            <v>22033008</v>
           </cell>
           <cell r="B65" t="str">
-            <v>名片-奥莱伊李</v>
+            <v>中型体力药剂</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>22036106</v>
+            <v>22033009</v>
           </cell>
           <cell r="B66" t="str">
-            <v>名片-米兰达</v>
+            <v>大型体力药剂</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>22036107</v>
+            <v>22033013</v>
           </cell>
           <cell r="B67" t="str">
-            <v>名片-盖露贝尔</v>
+            <v>随机幻兽卡</v>
           </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>22036108</v>
+            <v>22033014</v>
           </cell>
           <cell r="B68" t="str">
-            <v>名片-贝露凯伊鲁</v>
+            <v>随机武器卡</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>22036109</v>
+            <v>22033015</v>
           </cell>
           <cell r="B69" t="str">
-            <v>名片-雷洛比克</v>
+            <v>随机魔法卡</v>
           </cell>
         </row>
         <row r="70">
           <cell r="A70">
-            <v>22036110</v>
+            <v>22033016</v>
           </cell>
           <cell r="B70" t="str">
-            <v>名片-巴鲁迪亚斯</v>
+            <v>符文-查姆</v>
           </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>22036201</v>
+            <v>22033017</v>
           </cell>
           <cell r="B71" t="str">
-            <v>名片-武藤游戏</v>
+            <v>符文-普尔</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>22036202</v>
+            <v>22033018</v>
           </cell>
           <cell r="B72" t="str">
-            <v>名片-城之内</v>
+            <v>符文-艾尔</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>22036203</v>
+            <v>22033030</v>
           </cell>
           <cell r="B73" t="str">
-            <v>名片-海马懒人</v>
+            <v>木质修理锤</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>22036301</v>
+            <v>22033031</v>
           </cell>
           <cell r="B74" t="str">
-            <v>名片-内芙妮</v>
+            <v>钢铁修理锤</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>22036302</v>
+            <v>22033032</v>
           </cell>
           <cell r="B75" t="str">
-            <v>名片-塔妮丝</v>
+            <v>神圣修理锤</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>22036303</v>
+            <v>22034001</v>
           </cell>
           <cell r="B76" t="str">
-            <v>名片-卢卡</v>
+            <v>经验之书</v>
           </cell>
         </row>
         <row r="77">
           <cell r="A77">
-            <v>22036304</v>
+            <v>22034002</v>
           </cell>
           <cell r="B77" t="str">
-            <v>名片-艾斯特尔</v>
+            <v>能量之书</v>
           </cell>
         </row>
         <row r="78">
           <cell r="A78">
-            <v>22036305</v>
+            <v>22034003</v>
           </cell>
           <cell r="B78" t="str">
-            <v>名片-萨恩</v>
+            <v>攻速药水</v>
           </cell>
         </row>
         <row r="79">
           <cell r="A79">
-            <v>22036306</v>
+            <v>22034004</v>
           </cell>
           <cell r="B79" t="str">
-            <v>名片-玛莎</v>
+            <v>守护药水</v>
           </cell>
         </row>
         <row r="80">
           <cell r="A80">
-            <v>22036307</v>
+            <v>22034005</v>
           </cell>
           <cell r="B80" t="str">
-            <v>名片-阿特罗姆</v>
+            <v>法术药水</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>22036308</v>
+            <v>22034006</v>
           </cell>
           <cell r="B81" t="str">
-            <v>名片-泽诺</v>
+            <v>技巧药水</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>22036309</v>
+            <v>22034007</v>
           </cell>
           <cell r="B82" t="str">
-            <v>名片-拉凯尔</v>
+            <v>速度药水</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>22036310</v>
+            <v>22034008</v>
           </cell>
           <cell r="B83" t="str">
-            <v>名片-纳尔萨斯</v>
+            <v>幸运药水</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>22036311</v>
+            <v>22034009</v>
           </cell>
           <cell r="B84" t="str">
-            <v>名片-纳隆</v>
+            <v>暴击药水</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>22036312</v>
+            <v>22034010</v>
           </cell>
           <cell r="B85" t="str">
-            <v>名片-维加</v>
+            <v>饼干</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>22036401</v>
+            <v>22034011</v>
           </cell>
           <cell r="B86" t="str">
-            <v>名片-诺德</v>
+            <v>红色胶囊</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>22036402</v>
+            <v>22034012</v>
           </cell>
           <cell r="B87" t="str">
-            <v>名片-那那美</v>
+            <v>蓝色胶囊</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>22036403</v>
+            <v>22034013</v>
           </cell>
           <cell r="B88" t="str">
-            <v>名片-弗兰克</v>
+            <v>水晶球</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>22036404</v>
+            <v>22034014</v>
           </cell>
           <cell r="B89" t="str">
-            <v>名片-维克托</v>
+            <v>坐骑黑豹</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>22036405</v>
+            <v>22034015</v>
           </cell>
           <cell r="B90" t="str">
-            <v>名片-洛克</v>
+            <v>坐骑鹰</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>22036406</v>
+            <v>22034016</v>
           </cell>
           <cell r="B91" t="str">
-            <v>名片-谢拉</v>
+            <v>坐骑传送器</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22036407</v>
+            <v>22037001</v>
           </cell>
           <cell r="B92" t="str">
-            <v>名片-克莱布</v>
+            <v>种子-豌豆</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22036408</v>
+            <v>22037002</v>
           </cell>
           <cell r="B93" t="str">
-            <v>名片-蔡</v>
+            <v>种子-玉米</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22036501</v>
+            <v>22037003</v>
           </cell>
           <cell r="B94" t="str">
-            <v>名片-约修亚</v>
+            <v>种子-苹果</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22036502</v>
+            <v>22037004</v>
           </cell>
           <cell r="B95" t="str">
-            <v>名片-艾斯蒂尔</v>
+            <v>种子-蓝莓</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>22037001</v>
+            <v>22037101</v>
           </cell>
           <cell r="B96" t="str">
-            <v>种子-豌豆</v>
+            <v>作物-豌豆</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>22037002</v>
+            <v>22037102</v>
           </cell>
           <cell r="B97" t="str">
-            <v>种子-玉米</v>
+            <v>作物-玉米</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>22037003</v>
+            <v>22037103</v>
           </cell>
           <cell r="B98" t="str">
-            <v>种子-苹果</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99">
-            <v>22037004</v>
-          </cell>
-          <cell r="B99" t="str">
-            <v>种子-蓝莓</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100">
-            <v>22037101</v>
-          </cell>
-          <cell r="B100" t="str">
-            <v>作物-豌豆</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101">
-            <v>22037102</v>
-          </cell>
-          <cell r="B101" t="str">
-            <v>作物-豌豆</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102">
-            <v>22037103</v>
-          </cell>
-          <cell r="B102" t="str">
             <v>作物-苹果</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103">
-            <v>22037104</v>
-          </cell>
-          <cell r="B103" t="str">
-            <v>作物-蓝莓</v>
           </cell>
         </row>
       </sheetData>
@@ -1841,26 +1733,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:C21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:C21" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A3:C21"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" name="Item" dataDxfId="3"/>
-    <tableColumn id="3" name="~Name" dataDxfId="2"/>
+    <tableColumn id="1" name="Id" dataDxfId="2"/>
+    <tableColumn id="2" name="Item" dataDxfId="1"/>
+    <tableColumn id="3" name="~Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1928,6 +1820,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1963,6 +1872,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2142,11 +2068,12 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2192,7 +2119,7 @@
       </c>
       <c r="C4" s="7" t="str">
         <f>LOOKUP(TreasureWheel!$B4,[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>猛兽卡片</v>
+        <v>坐骑传送器</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -2288,7 +2215,7 @@
       </c>
       <c r="C12" s="7" t="str">
         <f>LOOKUP(TreasureWheel!$B12,[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>战斧卡片</v>
+        <v>坐骑传送器</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -2381,7 +2308,7 @@
       </c>
       <c r="C20" s="7" t="str">
         <f>LOOKUP(TreasureWheel!$B20,[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>体力药水</v>
+        <v>红色胶囊</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fix a tip bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/TreasureWheel.xlsx
+++ b/ConfigData/Xlsx/TreasureWheel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -88,7 +88,10 @@
     <t>hongsejiaonan</t>
   </si>
   <si>
-    <t>caishuijing</t>
+    <t>zyshi5</t>
+  </si>
+  <si>
+    <t>zyyu5</t>
   </si>
 </sst>
 </file>
@@ -799,7 +802,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -921,6 +924,20 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1272,7 +1289,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1446,7 +1463,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimise the wheel, support item count
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/TreasureWheel.xlsx
+++ b/ConfigData/Xlsx/TreasureWheel.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TreasureWheel" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -29,14 +29,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>宝物id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>Item</t>
   </si>
   <si>
     <t>string</t>
@@ -92,13 +85,253 @@
   </si>
   <si>
     <t>zyyu5</t>
+  </si>
+  <si>
+    <t>宝物id1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>宝物数量1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>宝物id2</t>
+  </si>
+  <si>
+    <t>宝物数量2</t>
+  </si>
+  <si>
+    <t>宝物id3</t>
+  </si>
+  <si>
+    <t>宝物数量3</t>
+  </si>
+  <si>
+    <t>宝物id4</t>
+  </si>
+  <si>
+    <t>宝物数量4</t>
+  </si>
+  <si>
+    <t>宝物id5</t>
+  </si>
+  <si>
+    <t>宝物数量5</t>
+  </si>
+  <si>
+    <t>宝物id6</t>
+  </si>
+  <si>
+    <t>宝物数量6</t>
+  </si>
+  <si>
+    <t>宝物id7</t>
+  </si>
+  <si>
+    <t>宝物数量7</t>
+  </si>
+  <si>
+    <t>宝物id8</t>
+  </si>
+  <si>
+    <t>宝物数量8</t>
+  </si>
+  <si>
+    <t>宝物id9</t>
+  </si>
+  <si>
+    <t>宝物数量9</t>
+  </si>
+  <si>
+    <t>宝物id10</t>
+  </si>
+  <si>
+    <t>宝物数量10</t>
+  </si>
+  <si>
+    <t>宝物id11</t>
+  </si>
+  <si>
+    <t>宝物数量11</t>
+  </si>
+  <si>
+    <t>宝物id12</t>
+  </si>
+  <si>
+    <t>宝物数量12</t>
+  </si>
+  <si>
+    <t>宝物id13</t>
+  </si>
+  <si>
+    <t>宝物数量13</t>
+  </si>
+  <si>
+    <t>宝物id14</t>
+  </si>
+  <si>
+    <t>宝物数量14</t>
+  </si>
+  <si>
+    <t>宝物id15</t>
+  </si>
+  <si>
+    <t>宝物数量15</t>
+  </si>
+  <si>
+    <t>宝物id16</t>
+  </si>
+  <si>
+    <t>宝物数量16</t>
+  </si>
+  <si>
+    <t>宝物id17</t>
+  </si>
+  <si>
+    <t>宝物数量17</t>
+  </si>
+  <si>
+    <t>宝物id18</t>
+  </si>
+  <si>
+    <t>宝物数量18</t>
+  </si>
+  <si>
+    <t>Item2</t>
+  </si>
+  <si>
+    <t>Count2</t>
+  </si>
+  <si>
+    <t>Item3</t>
+  </si>
+  <si>
+    <t>Count3</t>
+  </si>
+  <si>
+    <t>Item4</t>
+  </si>
+  <si>
+    <t>Count4</t>
+  </si>
+  <si>
+    <t>Item5</t>
+  </si>
+  <si>
+    <t>Count5</t>
+  </si>
+  <si>
+    <t>Item6</t>
+  </si>
+  <si>
+    <t>Count6</t>
+  </si>
+  <si>
+    <t>Item7</t>
+  </si>
+  <si>
+    <t>Count7</t>
+  </si>
+  <si>
+    <t>Item8</t>
+  </si>
+  <si>
+    <t>Count8</t>
+  </si>
+  <si>
+    <t>Item9</t>
+  </si>
+  <si>
+    <t>Count9</t>
+  </si>
+  <si>
+    <t>Item10</t>
+  </si>
+  <si>
+    <t>Count10</t>
+  </si>
+  <si>
+    <t>Item11</t>
+  </si>
+  <si>
+    <t>Count11</t>
+  </si>
+  <si>
+    <t>Item12</t>
+  </si>
+  <si>
+    <t>Count12</t>
+  </si>
+  <si>
+    <t>Item13</t>
+  </si>
+  <si>
+    <t>Count13</t>
+  </si>
+  <si>
+    <t>Item14</t>
+  </si>
+  <si>
+    <t>Count14</t>
+  </si>
+  <si>
+    <t>Item15</t>
+  </si>
+  <si>
+    <t>Count15</t>
+  </si>
+  <si>
+    <t>Item16</t>
+  </si>
+  <si>
+    <t>Count16</t>
+  </si>
+  <si>
+    <t>Item17</t>
+  </si>
+  <si>
+    <t>Count17</t>
+  </si>
+  <si>
+    <t>Item18</t>
+  </si>
+  <si>
+    <t>Count18</t>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>老</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +505,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -735,7 +976,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -756,6 +997,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -802,20 +1049,62 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -927,20 +1216,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -955,11 +1230,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:B21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A3:B21"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Id" dataDxfId="3"/>
-    <tableColumn id="2" name="Item" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:D4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A3:D4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E90684DF-74E0-40F0-ACAD-F6AF712A2213}" name="Name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Item1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{84322639-E92A-4268-81F6-795180163265}" name="Count1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1285,199 +1562,503 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9" customWidth="1"/>
+    <col min="4" max="4" width="4.375" customWidth="1"/>
+    <col min="6" max="6" width="4.625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.125" customWidth="1"/>
+    <col min="10" max="10" width="4.5" customWidth="1"/>
+    <col min="12" max="12" width="4.125" customWidth="1"/>
+    <col min="14" max="14" width="5" customWidth="1"/>
+    <col min="16" max="16" width="4.75" customWidth="1"/>
+    <col min="18" max="18" width="4.5" customWidth="1"/>
+    <col min="20" max="20" width="4.375" customWidth="1"/>
+    <col min="22" max="22" width="3.875" customWidth="1"/>
+    <col min="24" max="24" width="4.25" customWidth="1"/>
+    <col min="26" max="26" width="4.125" customWidth="1"/>
+    <col min="28" max="28" width="5" customWidth="1"/>
+    <col min="30" max="30" width="5" customWidth="1"/>
+    <col min="32" max="32" width="4.875" customWidth="1"/>
+    <col min="34" max="34" width="4.5" customWidth="1"/>
+    <col min="36" max="36" width="3.875" customWidth="1"/>
+    <col min="38" max="38" width="5.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:38" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>2</v>
+        <v>94</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>95</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>96</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ3" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL3" s="8" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="3">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="3">
-        <v>12</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="3">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="3">
-        <v>14</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="3">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="3">
-        <v>16</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="3">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+      <c r="AK4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="3">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
+      <c r="AL4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(B14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B21))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
add 2 new wheel datas
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/TreasureWheel.xlsx
+++ b/ConfigData/Xlsx/TreasureWheel.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="TreasureWheel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="154">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -36,9 +36,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>zuoqichuansongqi</t>
-  </si>
-  <si>
     <t>zhongxingmofayaoji</t>
   </si>
   <si>
@@ -79,12 +76,6 @@
   </si>
   <si>
     <t>hongsejiaonan</t>
-  </si>
-  <si>
-    <t>zyshi5</t>
-  </si>
-  <si>
-    <t>zyyu5</t>
   </si>
   <si>
     <t>宝物id1</t>
@@ -362,13 +353,157 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>zyshi6</t>
-  </si>
-  <si>
-    <t>zyyu6</t>
-  </si>
-  <si>
-    <t>new</t>
+    <t>kapaibugeibao(emo)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(jixie)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(jingling)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(kunchong)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(long)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(niao)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(paxing)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(renlei)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(shouren)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(wangling)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(yeshou)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(yu)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(yuansu)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(zhiwu)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(dijing)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(shixiang)</t>
+  </si>
+  <si>
+    <t>kapaibugeibao(shengwu)</t>
+  </si>
+  <si>
+    <t>生物卡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ziyuandai(emo)</t>
+  </si>
+  <si>
+    <t>ziyuandai(jixie)</t>
+  </si>
+  <si>
+    <t>ziyuandai(jingling)</t>
+  </si>
+  <si>
+    <t>ziyuandai(kunchong)</t>
+  </si>
+  <si>
+    <t>ziyuandai(long)</t>
+  </si>
+  <si>
+    <t>ziyuandai(niao)</t>
+  </si>
+  <si>
+    <t>ziyuandai(paxing)</t>
+  </si>
+  <si>
+    <t>ziyuandai(renlei)</t>
+  </si>
+  <si>
+    <t>ziyuandai(shouren)</t>
+  </si>
+  <si>
+    <t>ziyuandai(wangling)</t>
+  </si>
+  <si>
+    <t>ziyuandai(yeshou)</t>
+  </si>
+  <si>
+    <t>ziyuandai(yu)</t>
+  </si>
+  <si>
+    <t>ziyuandai(yuansu)</t>
+  </si>
+  <si>
+    <t>ziyuandai(zhiwu)</t>
+  </si>
+  <si>
+    <t>ziyuandai(dijing)</t>
+  </si>
+  <si>
+    <t>ziyuandai(shixiang)</t>
+  </si>
+  <si>
+    <t>sucaidaiteji</t>
+  </si>
+  <si>
+    <t>sucaidaijipin</t>
+  </si>
+  <si>
+    <t>素材</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>liuhuangbugeiche2</t>
+  </si>
+  <si>
+    <t>shuijingbugeiche2</t>
+  </si>
+  <si>
+    <t>hongbaoshibugeiche2</t>
+  </si>
+  <si>
+    <t>shuiyinbugeiche2</t>
+  </si>
+  <si>
+    <t>mucaibugeiche2</t>
+  </si>
+  <si>
+    <t>kuangshibugeiche2</t>
+  </si>
+  <si>
+    <t>zuoqiheibao</t>
+  </si>
+  <si>
+    <t>zuoqiying</t>
+  </si>
+  <si>
+    <t>lansejiaonan</t>
+  </si>
+  <si>
+    <t>binggan</t>
+  </si>
+  <si>
+    <t>WheelBack2</t>
+  </si>
+  <si>
+    <t>WheelBack3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1033,7 +1168,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1048,6 +1183,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -2304,8 +2442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AO5" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
-  <autoFilter ref="A3:AO5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AO7" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+  <autoFilter ref="A3:AO7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="40"/>
     <tableColumn id="4" xr3:uid="{E90684DF-74E0-40F0-ACAD-F6AF712A2213}" name="Name" dataDxfId="37"/>
@@ -2674,15 +2812,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO5"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="9" customWidth="1"/>
+    <col min="1" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
     <col min="7" max="7" width="4.375" customWidth="1"/>
     <col min="9" max="9" width="4.625" customWidth="1"/>
     <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
@@ -2705,378 +2844,378 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>102</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="AM1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO1" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>96</v>
+      <c r="B2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AJ2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AN2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.15">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>104</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="L3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="N3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="P3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="R3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="T3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="V3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="W3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="X3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="Z3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="AB3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AD3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AE3" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AF3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AD3" s="7" t="s">
+      <c r="AG3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AH3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AF3" s="7" t="s">
+      <c r="AI3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="AH3" s="7" t="s">
+      <c r="AK3" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AL3" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AJ3" s="7" t="s">
+      <c r="AM3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="AK3" s="6" t="s">
+      <c r="AN3" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="AL3" s="7" t="s">
+      <c r="AO3" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="AO3" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.15">
@@ -3084,7 +3223,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3093,114 +3232,114 @@
         <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="6">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5">
-        <v>1</v>
-      </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="6">
+        <v>2</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="5">
-        <v>2</v>
-      </c>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="5">
-        <v>1</v>
-      </c>
-      <c r="R4" s="5" t="s">
+      <c r="S4" s="6">
+        <v>1</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="5">
-        <v>1</v>
-      </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="6">
+        <v>1</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="W4" s="6">
+        <v>1</v>
+      </c>
+      <c r="X4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="5">
-        <v>1</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="W4" s="5">
-        <v>1</v>
-      </c>
-      <c r="X4" s="5" t="s">
+      <c r="Y4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Y4" s="5">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="5" t="s">
+      <c r="AC4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="AC4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="5" t="s">
+      <c r="AE4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AE4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="5" t="s">
+      <c r="AG4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="5" t="s">
+      <c r="AI4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AI4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="5" t="s">
+      <c r="AK4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AK4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM4" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AO4" s="5">
+      <c r="AM4" s="6">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="AO4" s="6">
         <v>1</v>
       </c>
     </row>
@@ -3209,7 +3348,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -3218,115 +3357,365 @@
         <v>200</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5">
-        <v>2</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="5">
-        <v>2</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="5">
-        <v>2</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="5">
-        <v>3</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>2</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="5">
-        <v>2</v>
+        <v>104</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="S5" s="6">
+        <v>1</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="U5" s="5">
         <v>2</v>
       </c>
       <c r="V5" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="W5" s="5">
+        <v>1</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO5" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="5">
+        <v>1</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>1</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="S6" s="5">
+        <v>1</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="U6" s="5">
+        <v>1</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="W6" s="5">
+        <v>1</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="W5" s="5">
-        <v>2</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y5" s="5">
-        <v>2</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AD5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AF5" s="5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>1</v>
+      </c>
+      <c r="R7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AG5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AH5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AJ5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AL5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM5" s="5">
-        <v>2</v>
-      </c>
-      <c r="AN5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AO5" s="5">
-        <v>2</v>
+      <c r="S7" s="5">
+        <v>1</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="5">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="W7" s="5">
+        <v>1</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO7" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>